<commit_message>
newst data without dates
</commit_message>
<xml_diff>
--- a/testdata/TimeWire_Events_and_Articles_Spreadsheet.xlsx
+++ b/testdata/TimeWire_Events_and_Articles_Spreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="-40" windowWidth="24800" windowHeight="16020" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="540" yWindow="-40" windowWidth="24800" windowHeight="16040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Articles" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,139 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="233">
+  <si>
+    <t>syria_US_journalist_still_missing/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>attack_on_syria_would_be/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Israeli_warplanes_research_center/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Turkey_shelters_anti_assad/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>syria_reports_of_heavy_firefight/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>7_dead_as_syrian_troops/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>turkey_renews_shelling_of_syrian/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>syrian_opposition_fails_to_form/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>attack_on_syria_would_be/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>activists_killed_as_wounded/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>footage_of_torture_emerges/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>syria_reports_of_heavy_firefight/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>7_dead_as_syrian_troops/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>syrians_crisis_UN_mission/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>more_than_300_bodies_found/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>syrias_rebels_claim_capture</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>syria_crisis_aleppo_rebels/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>syria_rebels_kill_7/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>bashar_as-assad_calls_for_dialogue/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>turkey_renews_shelling_of_syrian/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>syria_and_the_battle_for_regional_control</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>assad_replies_to_syria_ceasefire</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>syria_rebels_advance_in_aleppo/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>israel_fires_warning_shots_into_syria/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>turks_grant_recognition_to_coalition/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>syria_launches_air_strikes/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>un_envoy_is_seeking_deal_to_oust/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>syrian_rebel_army_set/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>kidnapped_NBC_journalist_freed/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>aleppos_attorney_general_defects/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>syrias_bashar_al_assad_calls/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>french_journalist_killed/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>syrian_opposition_fails_to_form/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
   <si>
     <t>Greece, Crisis, Financial, Tax, Strike, Austerity</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -34,7 +166,35 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>2012_10_25/syria_rebels_advance_in_aleppo/</t>
+    <t>scores_arrested_as_syrian/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>syria_conflict_mortars/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>syrians_abroad_report_harassment/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Turkey_shelters_anti_assad/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>syria_mining_border_with_Lebanon/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>arab_league_sanctions_for_syria</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>violent_protests_outside_syrian_embassy/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>obituary_syrian_citizen_journalist/</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -46,34 +206,14 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>2012_12_11/syrian_rebel_army_set/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Syria, Conflict, Rebel, Opposition</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>2012_12_27/aleppos_attorney_general_defects/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Syria, Conflict, Aleppo, Defection</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>2013_01_06/syrias_bashar_al_assad_calls/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2013_01_18/french_journalist_killed/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2013_01_26/attack_on_syria_would_be/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Syria, Conflict, Iran, Attack</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -118,54 +258,26 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>2011_05_09/scores_arrested_as_syrian/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Syria, Conflict, Protests, Assad</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>2011_08_03/syria_conflict_mortars/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Syria, Conflict, Damascus, Assad, Refugee, Palestine</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>2011_10_03/syrians_abroad_report_harassment/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Syria, Conflict, World, Expat</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>2011_10_28/Turkey_shelters_anti_assad/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Syria, Turkey, Anti-Assad, Free Syrian Army</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>2011_11_01/syria_mining_border_with_Lebanon/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Syria, Conflict, Lebanon, Border</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>2011_11_12/arab_league_sanctions_for_syria</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2012_02_04/violent_protests_outside_syrian_embassy/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Syria, London, Protest</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -182,78 +294,38 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>2012_03_19/syria_reports_of_heavy_firefight/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Syria, Conflict, Damascus, War, Free Syrian Army</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>2012_05_02/7_dead_as_syrian_troops/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Syria, Conflict, Syrian Troops, Aleppo, University, Students</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>2012_07_20/syrians_crisis_UN_mission/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Syria, Conflict, Damascus, Refugee, UN</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>2012_08_26/more_than_300_bodies_found/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2012_08_29/syrias_rebels_claim_capture</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Syria, Conflict, Free Syrian Army, Weapons, Damascus, Rebels</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>2012_09_06/syria_crisis_aleppo_rebels/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Syria, Conflict, Free Syrian Army, Aleppo, Rebels</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>2012_09_09/syria_rebels_kill_7/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Syria, Conflict, Assad, Dialogue, UN</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>2012_10_16/syria_and_the_battle_for_regional_control</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Syria, Conflict, Russia, Turkey, Assad, US</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>2012_10_24/assad_replies_to_syria_ceasefire</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Syria, Conflict, Assad, Ceasefire, Air Strikes</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>2013_01_21/syrian_opposition_fails_to_form/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Syria, Conflict, Opposition, Rebels</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -264,13 +336,6 @@
     <t>Syria: US journalist still missing</t>
   </si>
   <si>
-    <t>2013_01_23/syria_US_journalist_still_missing/</t>
-  </si>
-  <si>
-    <t>2013_01_23/syria_US_journalist_still_missing/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Syria, Conflict, US, Journalist</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -281,10 +346,6 @@
     <t>http://en-maktoob.news.yahoo.com/family-appeals-release-reporter-kidnapped-syria-223656369.html</t>
   </si>
   <si>
-    <t>2013_01_23/syria_US_journalist_still_missing/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>http://www.youtube.com/watch?v=tf0QOS_tV1M</t>
   </si>
   <si>
@@ -297,20 +358,12 @@
     <t>Attack on Syria would be seen as attack on Iran</t>
   </si>
   <si>
-    <t>2013_01_26/attack_on_syria_would_be/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>http://rt.com/news/israeli-warplanes-bomb-damascus-114/</t>
   </si>
   <si>
     <t>Israeli warplanes bomb research center near Damascus - Syrian military</t>
   </si>
   <si>
-    <t>2013_01_30/Israeli_warplanes_research_center/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Syria, Conflict, Israel, Attack, Damascus</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -348,10 +401,6 @@
     <t>Aleppo’s attorney-general defects, denounces Syrian regime’s ‘crimes’</t>
   </si>
   <si>
-    <t>2012_12_27/aleppos_attorney_general_defects/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>http://www.reuters.com/article/2012/12/27/us-syria-crisis-idUSBRE8AJ1FK20121227</t>
   </si>
   <si>
@@ -361,10 +410,6 @@
     <t>Syria's Bashar al-Assad calls on foreign countries to end support for rebels</t>
   </si>
   <si>
-    <t>2013_01_06/syrias_bashar_al_assad_calls/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Syria, Conflict, Assad, World, Rebels</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -387,13 +432,6 @@
     <t>French journalist killed by sniper fire in Syria</t>
   </si>
   <si>
-    <t>2013_01_18/french_journalist_killed/</t>
-  </si>
-  <si>
-    <t>2013_01_18/french_journalist_killed/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Syria, Conflict, France, Journalist, Death</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -414,10 +452,6 @@
     <t>Syrian opposition fails to form transitional government</t>
   </si>
   <si>
-    <t>2012_11_27/syria_launches_air_strikes/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>http://blogs.aljazeera.com/topic/syria/video-shows-long-lines-people-waiting-get-bread-aleppo</t>
   </si>
   <si>
@@ -427,10 +461,6 @@
     <t>http://www.nytimes.com/2012/12/07/world/middleeast/us-and-russia-to-meet-on-syrian-conflict.html?gwh=25D5E8218BC9E8B8F8E06C840F5BB72D</t>
   </si>
   <si>
-    <t>2012_12_06/un_envoy_is_seeking_deal_to_oust/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>http://www.independent.co.uk/news/world/middle-east/exclusive-uk-military-in-talks-to-help-syria-rebels-8399658.html</t>
   </si>
   <si>
@@ -443,20 +473,12 @@
     <t>Syrian Rebel Army Set to Join New Opposition Group</t>
   </si>
   <si>
-    <t>2012_12_11/syrian_rebel_army_set/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>http://www.guardian.co.uk/media/greenslade/2012/dec/18/journalist-safety-syria</t>
   </si>
   <si>
     <t>Kidnapped NBC journalist freed after firefight in Syria</t>
   </si>
   <si>
-    <t>2012_12_18/kidnapped_NBC_journalist_freed/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Syria, Conflict, Journalist, US</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -473,10 +495,6 @@
     <t>Syria rebels 'advance in Aleppo'</t>
   </si>
   <si>
-    <t>2012_10_25/syria_rebels_advance_in_aleppo/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>http://www.guardian.co.uk/world/2012/nov/11/israel-fires-missile-into-syria</t>
   </si>
   <si>
@@ -486,10 +504,6 @@
     <t>Israel Fires Warning Shots Into Syria</t>
   </si>
   <si>
-    <t>2012_11_11/israel_fires_warning_shots_into_syria/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Syria, Conflict, Free Syrian Army, Aleppo, Rebels</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -507,10 +521,6 @@
     <t>Turks Grant Recognition to Coalition of Syrians</t>
   </si>
   <si>
-    <t>2012_11_15/turks_grant_recognition_to_coalition/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Syria, Conflict, Turkey, Free Syrian Army, Rebels</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -533,10 +543,6 @@
     <t>Syria launches air strikes as combat rages in Damascus</t>
   </si>
   <si>
-    <t>2012_10_04/turkey_renews_shelling_of_syrian/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Syria, Conflict, Turkey, War, Syrian Army</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -547,18 +553,10 @@
     <t>More than 300 bodies found in Syrian town of Darya</t>
   </si>
   <si>
-    <t>2012_08_26/more_than_300_bodies_found/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Syria, Conflict, Daraya, Assad</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>2012_09_09/syria_rebels_kill_7/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>http://www.globalpost.com/dispatch/news/regions/middle-east/syria/120826/inside-syria-sunday-massacre-daraya-assad-regime-brin</t>
   </si>
   <si>
@@ -571,10 +569,6 @@
     <t>Syria and the battle for regional control</t>
   </si>
   <si>
-    <t>2012_10_16/syria_and_the_battle_for_regional_control</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>http://www.turkishweekly.net/news/143656/us-urges-russia-to-take-more-action-on-syria.html</t>
   </si>
   <si>
@@ -593,10 +587,6 @@
     <t>Assad replies to Syria ceasefire call with air strikes</t>
   </si>
   <si>
-    <t>2012_10_24/assad_replies_to_syria_ceasefire</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Syria rebels kill 7, bomb explodes near U.N. monitors</t>
   </si>
   <si>
@@ -613,10 +603,6 @@
     <t>http://www.presstv.ir/detail/2012/09/15/261700/assad-urges-dialogue-between-syrians/</t>
   </si>
   <si>
-    <t>2012_9_15/bashar_as-assad_calls_for_dialogue/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>http://www.reuters.com/article/2012/09/15/us-syria-crisis-assad-idUSBRE88E03U20120915</t>
   </si>
   <si>
@@ -638,10 +624,6 @@
     <t>http://www.dailystar.com.lb/News/Middle-East/2012/May-04/172322-un-mission-chief-says-syria-army-must-cease-fire-first.ashx#axzz2KKgPcvJh</t>
   </si>
   <si>
-    <t>2012_05_02/7_dead_as_syrian_troops/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>http://www.arabnews.com/syria%E2%80%99s-rebels-claim-capture-missiles-damascus</t>
   </si>
   <si>
@@ -666,24 +648,12 @@
     <t>Syria crisis: Aleppo rebels vow to fight on</t>
   </si>
   <si>
-    <t>2012_09_06/syria_crisis_aleppo_rebels/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2012_03_06/footage_of_torture_emerges/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>http://www.guardian.co.uk/world/2012/mar/19/syria-damascus-firefight-reports</t>
   </si>
   <si>
     <t>Syria: reports of heavy firefight in western Damascus</t>
   </si>
   <si>
-    <t>2012_03_19/syria_reports_of_heavy_firefight/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>http://edition.cnn.com/2012/03/19/world/meast/syria-unrest</t>
   </si>
   <si>
@@ -706,10 +676,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>2012_07_20/syrians_crisis_UN_mission/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>http://edition.cnn.com/2012/05/03/world/meast/syria-unrest</t>
   </si>
   <si>
@@ -722,10 +688,6 @@
     <t>'Activists killed' as wounded photographer smuggled out of Syria</t>
   </si>
   <si>
-    <t>2012_02_29/activists_killed_as_wounded/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Syria, Conflict, Arab League, Sanctions</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -756,20 +718,12 @@
     <t>Syria mining border with Lebanon</t>
   </si>
   <si>
-    <t>2011_11_01/syria_mining_border_with_Lebanon/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>http://www.bbc.co.uk/news/world-middle-east-15706851</t>
   </si>
   <si>
     <t>Arab League sanctions for Syria</t>
   </si>
   <si>
-    <t>2011_11_12/arab_league_sanctions_for_syria</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>http://www.telegraph.co.uk/news/worldnews/middleeast/syria/8892093/Why-did-the-Arab-League-tyrants-club-finally-turn-on-Syria.html</t>
   </si>
   <si>
@@ -792,20 +746,12 @@
     <t>Violent protests outside Syrian embassy in London over 'massacre'</t>
   </si>
   <si>
-    <t>2012_02_04/violent_protests_outside_syrian_embassy/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>http://www.bbc.co.uk/news/world-middle-east-17131958</t>
   </si>
   <si>
     <t>Obituary: Syrian citizen journalist Rami al-Sayed</t>
   </si>
   <si>
-    <t>2012_02_22/obituary_syrian_citizen_journalist/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>http://www.huffingtonpost.com/2012/02/22/rami-al-sayed-dead-syrian-blogger-homs_n_1293853.html</t>
   </si>
   <si>
@@ -824,10 +770,6 @@
     <t>http://articles.latimes.com/2011/may/09/world/la-fg-syria-arrests-20110510</t>
   </si>
   <si>
-    <t>2011_05_09/scores_arrested_as_syrian/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>http://blog.amnestyusa.org/middle-east/repression-goes-global-syrians-in-us-targeted-by-syrian-embassies/</t>
   </si>
   <si>
@@ -840,10 +782,6 @@
     <t>http://thelede.blogs.nytimes.com/2011/10/03/syrians-abroad-report-harassment-and-intimidation/</t>
   </si>
   <si>
-    <t>2011_10_03/syrians_abroad_report_harassment/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>http://www.globalpost.com/dispatch/news/regions/europe/turkey/111027/turkey-free-syrian-army-syria</t>
   </si>
   <si>
@@ -856,10 +794,6 @@
     <t>Turkey Shelters Anti-Assad Group, the Free Syrian Army</t>
   </si>
   <si>
-    <t>2011_10_28/Turkey_shelters_anti_assad/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>http://news.yahoo.com/syria-mining-border-lebanon-165919478.html</t>
   </si>
   <si>
@@ -876,10 +810,6 @@
   </si>
   <si>
     <t>Syria Conflict: Mortars Hit Palestinian Refugee Camp In Damascus, At Least 20 Killed</t>
-  </si>
-  <si>
-    <t>2012_08_03/syria_conflict-mortars/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>http://www.nytimes.com/2011/09/17/world/middleeast/at-least-six-protesters-killed-in-syria.html?pagewanted=1&amp;_r=1</t>
@@ -1387,8 +1317,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C128"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="H110" sqref="A105:H110"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="C110" sqref="C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1398,922 +1328,928 @@
   <sheetData>
     <row r="1" spans="1:3" s="5" customFormat="1">
       <c r="B1" s="8" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="52">
       <c r="B2" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="C2" t="s">
-        <v>249</v>
+        <v>228</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="65">
       <c r="B3" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="C3" t="s">
-        <v>249</v>
+        <v>230</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="65">
       <c r="A4" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="C4" t="s">
-        <v>249</v>
+        <v>229</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="39">
       <c r="B5" s="1" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="C5" t="s">
-        <v>232</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="65">
       <c r="B6" s="1" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="C6" t="s">
-        <v>232</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="39">
       <c r="A7" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="C7" t="s">
-        <v>232</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="52">
       <c r="B8" s="1" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="C8" t="s">
-        <v>237</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="52">
       <c r="B9" s="1" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="C9" t="s">
-        <v>237</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="52">
       <c r="A10" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="C10" t="s">
-        <v>237</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="52">
       <c r="B11" s="1" t="s">
-        <v>238</v>
+        <v>222</v>
       </c>
       <c r="C11" t="s">
-        <v>242</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="39">
       <c r="B12" s="1" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="C12" t="s">
-        <v>242</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="26">
       <c r="A13" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
       <c r="C13" t="s">
-        <v>242</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="52">
       <c r="B14" s="1" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="C14" t="s">
-        <v>211</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="52">
       <c r="B15" s="1" t="s">
-        <v>244</v>
+        <v>227</v>
       </c>
       <c r="C15" t="s">
-        <v>211</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="39">
       <c r="A16" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
       <c r="C16" t="s">
-        <v>211</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="39">
       <c r="B17" s="1" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="C17" t="s">
-        <v>214</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="65">
       <c r="B18" s="1" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="C18" t="s">
-        <v>214</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="26">
       <c r="A19" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="C19" t="s">
-        <v>214</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="26">
       <c r="B20" s="1" t="s">
-        <v>218</v>
+        <v>206</v>
+      </c>
+      <c r="C20" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="39">
       <c r="B21" s="1" t="s">
-        <v>217</v>
+        <v>205</v>
+      </c>
+      <c r="C21" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="65">
       <c r="A22" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C22" t="s">
-        <v>222</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="52">
       <c r="B23" s="1" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="C23" t="s">
-        <v>225</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="52">
       <c r="B24" s="1" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="C24" t="s">
-        <v>225</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="26">
       <c r="A25" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="C25" t="s">
-        <v>225</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="52">
       <c r="B26" s="1" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="C26" t="s">
-        <v>201</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="39">
       <c r="B27" s="1" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="C27" t="s">
-        <v>201</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="52">
       <c r="A28" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="C28" t="s">
-        <v>201</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="39">
       <c r="B29" s="1" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="C29" t="s">
-        <v>185</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="52">
       <c r="B30" s="1" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C30" t="s">
-        <v>185</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="26">
       <c r="A31" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="C31" t="s">
-        <v>185</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="26">
       <c r="B32" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="C32" t="s">
-        <v>188</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="26">
       <c r="B33" s="1" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="C33" t="s">
-        <v>188</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="39">
       <c r="A34" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="C34" t="s">
-        <v>188</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="65">
       <c r="B35" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C35" t="s">
-        <v>175</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="65">
       <c r="B36" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C36" t="s">
-        <v>175</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="26">
       <c r="A37" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="C37" t="s">
-        <v>175</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="78">
       <c r="B38" s="1" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="C38" t="s">
-        <v>196</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="39">
       <c r="B39" s="1" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="C39" t="s">
-        <v>196</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="52">
       <c r="A40" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="C40" t="s">
-        <v>196</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="39">
       <c r="B41" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C41" t="s">
-        <v>147</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="65">
       <c r="B42" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C42" t="s">
-        <v>147</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="26">
       <c r="A43" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C43" t="s">
-        <v>147</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="65">
       <c r="B44" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C44" t="s">
-        <v>184</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="39">
       <c r="B45" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C45" t="s">
-        <v>184</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="52">
       <c r="A46" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C46" t="s">
-        <v>184</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="39">
       <c r="B47" s="1" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C47" t="s">
-        <v>149</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="26">
       <c r="B48" s="1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C48" t="s">
-        <v>149</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="39">
       <c r="A49" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C49" t="s">
-        <v>149</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="52">
       <c r="B50" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C50" t="s">
-        <v>167</v>
+        <v>18</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="52">
       <c r="B51" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C51" t="s">
-        <v>167</v>
+        <v>18</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="60">
       <c r="A52" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C52" t="s">
-        <v>167</v>
+        <v>18</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="39">
       <c r="B53" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C53" t="s">
-        <v>143</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="26">
       <c r="B54" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C54" t="s">
-        <v>143</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="52">
       <c r="A55" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C55" t="s">
-        <v>143</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="39">
       <c r="B56" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C56" t="s">
-        <v>154</v>
+        <v>20</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="39">
       <c r="B57" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C57" t="s">
-        <v>154</v>
+        <v>20</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="39">
       <c r="A58" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C58" t="s">
-        <v>154</v>
+        <v>20</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="52">
       <c r="B59" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C59" t="s">
-        <v>161</v>
+        <v>21</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="52">
       <c r="B60" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C60" t="s">
-        <v>161</v>
+        <v>21</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="52">
       <c r="A61" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C61" t="s">
-        <v>161</v>
+        <v>21</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="39">
       <c r="B62" s="1" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="C62" t="s">
-        <v>125</v>
+        <v>22</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="52">
       <c r="B63" s="1" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="C63" t="s">
-        <v>125</v>
+        <v>22</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="26">
       <c r="A64" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C64" t="s">
-        <v>125</v>
+        <v>22</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="39">
       <c r="B65" s="1" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C65" t="s">
-        <v>129</v>
+        <v>23</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="26">
       <c r="B66" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C66" t="s">
-        <v>129</v>
+        <v>23</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="39">
       <c r="A67" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C67" t="s">
-        <v>129</v>
+        <v>23</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="39">
       <c r="B68" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C68" t="s">
-        <v>135</v>
+        <v>24</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="26">
       <c r="B69" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C69" t="s">
-        <v>135</v>
+        <v>24</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="65">
       <c r="A70" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C70" t="s">
-        <v>135</v>
+        <v>24</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="52">
       <c r="B71" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C71" t="s">
-        <v>107</v>
+        <v>25</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="39">
       <c r="B72" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C72" t="s">
-        <v>107</v>
+        <v>25</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="39">
       <c r="A73" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C73" t="s">
-        <v>107</v>
+        <v>25</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="52">
       <c r="B74" s="1" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="C74" t="s">
-        <v>111</v>
+        <v>26</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="39">
       <c r="B75" s="1" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="C75" t="s">
-        <v>111</v>
+        <v>26</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="65">
       <c r="A76" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="C76" t="s">
-        <v>111</v>
+        <v>26</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="65">
       <c r="B77" s="1" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="C77" t="s">
-        <v>116</v>
+        <v>27</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="26">
       <c r="B78" s="1" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="C78" t="s">
-        <v>116</v>
+        <v>27</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="52">
       <c r="A79" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="C79" t="s">
-        <v>116</v>
+        <v>27</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="26">
       <c r="B80" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="C80" t="s">
-        <v>119</v>
+        <v>28</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="26">
       <c r="B81" s="1" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="C81" t="s">
-        <v>119</v>
+        <v>28</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="39">
       <c r="A82" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="C82" t="s">
-        <v>119</v>
+        <v>28</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="39">
       <c r="B83" s="1" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="C83" t="s">
-        <v>87</v>
+        <v>29</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="39">
       <c r="B84" s="1" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C84" t="s">
-        <v>87</v>
+        <v>29</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="26">
       <c r="A85" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="C85" t="s">
-        <v>87</v>
+        <v>29</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="52">
       <c r="B86" s="1" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="C86" t="s">
-        <v>91</v>
+        <v>30</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="39">
       <c r="B87" s="1" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="C87" t="s">
-        <v>91</v>
+        <v>30</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="39">
       <c r="A88" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C88" t="s">
-        <v>91</v>
+        <v>30</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="39">
       <c r="B89" s="1" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="C89" t="s">
-        <v>100</v>
+        <v>31</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="26">
       <c r="B90" s="1" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="C90" t="s">
-        <v>100</v>
+        <v>31</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="52">
       <c r="A91" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="C91" t="s">
-        <v>99</v>
+        <v>31</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="39">
       <c r="B92" s="1" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="C92" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="52">
       <c r="B93" s="1" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="C93" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="52">
       <c r="A94" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="C94" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="65">
       <c r="B95" s="1" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="C95" t="s">
-        <v>63</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="52">
       <c r="B96" s="1" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="C96" t="s">
-        <v>67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="52">
       <c r="A97" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="C97" t="s">
-        <v>62</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="26">
       <c r="B98" s="1" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="C98" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="52">
       <c r="B99" s="1" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="C99" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="39">
       <c r="A100" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="C100" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="39">
       <c r="B101" s="1" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="C101" t="s">
-        <v>75</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="52">
       <c r="B102" s="1" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="C102" t="s">
-        <v>75</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="39">
       <c r="A103" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C103" t="s">
-        <v>75</v>
+        <v>2</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -2327,20 +2263,20 @@
     </row>
     <row r="126" spans="1:2" ht="39">
       <c r="B126" s="1" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="78">
       <c r="B127" s="1" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="39">
       <c r="A128" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -2361,8 +2297,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -2376,27 +2312,27 @@
   <sheetData>
     <row r="1" spans="1:6" s="5" customFormat="1">
       <c r="A1" s="3" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="10" customFormat="1">
       <c r="A3" s="22" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="B3" s="9">
         <v>39302</v>
@@ -2405,10 +2341,10 @@
         <v>39302.999988425923</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="F3" s="10">
         <v>50</v>
@@ -2416,7 +2352,7 @@
     </row>
     <row r="4" spans="1:6" s="10" customFormat="1" ht="16" customHeight="1">
       <c r="A4" s="22" t="s">
-        <v>248</v>
+        <v>231</v>
       </c>
       <c r="B4" s="9">
         <v>39296</v>
@@ -2425,10 +2361,10 @@
         <v>39297.999988425923</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="F4" s="10">
         <v>70</v>
@@ -2436,7 +2372,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="22" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="B5" s="11">
         <v>39357</v>
@@ -2445,10 +2381,10 @@
         <v>39358.999988425923</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="F5" s="12">
         <v>30</v>
@@ -2456,7 +2392,7 @@
     </row>
     <row r="6" spans="1:6" s="14" customFormat="1">
       <c r="A6" s="23" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="B6" s="13">
         <v>39382</v>
@@ -2465,10 +2401,10 @@
         <v>39382.999988425923</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="F6" s="12">
         <v>80</v>
@@ -2476,7 +2412,7 @@
     </row>
     <row r="7" spans="1:6" s="16" customFormat="1">
       <c r="A7" s="24" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="B7" s="15">
         <v>39386</v>
@@ -2485,10 +2421,10 @@
         <v>39386.999988425923</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="F7" s="12">
         <v>72</v>
@@ -2496,7 +2432,7 @@
     </row>
     <row r="8" spans="1:6" s="14" customFormat="1">
       <c r="A8" s="24" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="B8" s="13">
         <v>39397</v>
@@ -2505,10 +2441,10 @@
         <v>39397.999988425923</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="F8" s="14">
         <v>90</v>
@@ -2516,7 +2452,7 @@
     </row>
     <row r="9" spans="1:6" s="18" customFormat="1">
       <c r="A9" s="24" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="B9" s="17">
         <v>39481</v>
@@ -2525,10 +2461,10 @@
         <v>39481.999884259261</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="F9" s="14">
         <v>40</v>
@@ -2536,7 +2472,7 @@
     </row>
     <row r="10" spans="1:6" s="14" customFormat="1">
       <c r="A10" s="24" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="B10" s="13">
         <v>39499</v>
@@ -2545,10 +2481,10 @@
         <v>39499.999988425923</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>225</v>
+        <v>43</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="F10" s="14">
         <v>60</v>
@@ -2556,7 +2492,7 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="23" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="B11" s="11">
         <v>39506</v>
@@ -2565,10 +2501,10 @@
         <v>39506.999988425923</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>201</v>
+        <v>9</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="F11" s="14">
         <v>45</v>
@@ -2576,7 +2512,7 @@
     </row>
     <row r="12" spans="1:6" s="14" customFormat="1" ht="17" customHeight="1">
       <c r="A12" s="24" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="B12" s="13">
         <v>39512</v>
@@ -2585,10 +2521,10 @@
         <v>39512.999988425923</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>185</v>
+        <v>10</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="F12" s="14">
         <v>70</v>
@@ -2596,7 +2532,7 @@
     </row>
     <row r="13" spans="1:6" s="18" customFormat="1" ht="13" customHeight="1">
       <c r="A13" s="24" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B13" s="17">
         <v>39525</v>
@@ -2605,10 +2541,10 @@
         <v>39525.999988425923</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="F13" s="14">
         <v>80</v>
@@ -2616,7 +2552,7 @@
     </row>
     <row r="14" spans="1:6" s="16" customFormat="1">
       <c r="A14" s="22" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="B14" s="15">
         <v>39569</v>
@@ -2625,10 +2561,10 @@
         <v>39569.999988425923</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="F14" s="14">
         <v>90</v>
@@ -2636,7 +2572,7 @@
     </row>
     <row r="15" spans="1:6" s="18" customFormat="1">
       <c r="A15" s="24" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="B15" s="17">
         <v>39648</v>
@@ -2645,10 +2581,10 @@
         <v>39648.999988425923</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="F15" s="14">
         <v>90</v>
@@ -2656,7 +2592,7 @@
     </row>
     <row r="16" spans="1:6" s="14" customFormat="1">
       <c r="A16" s="24" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B16" s="13">
         <v>39685</v>
@@ -2665,7 +2601,7 @@
         <v>39685.999988425923</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="E16" s="14" t="s">
         <v>148</v>
@@ -2676,7 +2612,7 @@
     </row>
     <row r="17" spans="1:6" s="10" customFormat="1">
       <c r="A17" s="24" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B17" s="9">
         <v>39688</v>
@@ -2685,10 +2621,10 @@
         <v>39688.999988425923</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="F17" s="14">
         <v>85</v>
@@ -2696,7 +2632,7 @@
     </row>
     <row r="18" spans="1:6" s="18" customFormat="1">
       <c r="A18" s="24" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B18" s="17">
         <v>39696</v>
@@ -2705,10 +2641,10 @@
         <v>39696.999988425923</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="F18" s="14">
         <v>80</v>
@@ -2716,7 +2652,7 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="24" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B19" s="11">
         <v>39699</v>
@@ -2725,10 +2661,10 @@
         <v>39699.999988425923</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F19" s="14">
         <v>85</v>
@@ -2736,7 +2672,7 @@
     </row>
     <row r="20" spans="1:6" s="16" customFormat="1">
       <c r="A20" s="23" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B20" s="15">
         <v>39705</v>
@@ -2745,10 +2681,10 @@
         <v>39705.999988425923</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>167</v>
+        <v>18</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="F20" s="14">
         <v>95</v>
@@ -2756,7 +2692,7 @@
     </row>
     <row r="21" spans="1:6" s="18" customFormat="1">
       <c r="A21" s="24" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B21" s="17">
         <v>39724</v>
@@ -2765,10 +2701,10 @@
         <v>39724.999988425923</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>143</v>
+        <v>19</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F21" s="14">
         <v>75</v>
@@ -2776,7 +2712,7 @@
     </row>
     <row r="22" spans="1:6" s="18" customFormat="1">
       <c r="A22" s="24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B22" s="17">
         <v>39736</v>
@@ -2785,10 +2721,10 @@
         <v>39736.999988425923</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="F22" s="14">
         <v>60</v>
@@ -2796,7 +2732,7 @@
     </row>
     <row r="23" spans="1:6" s="18" customFormat="1">
       <c r="A23" s="22" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B23" s="17">
         <v>39744</v>
@@ -2805,10 +2741,10 @@
         <v>39744.999988425923</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="F23" s="14">
         <v>92</v>
@@ -2816,7 +2752,7 @@
     </row>
     <row r="24" spans="1:6" s="14" customFormat="1">
       <c r="A24" s="24" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="B24" s="13">
         <v>39745</v>
@@ -2825,10 +2761,10 @@
         <v>39745.999988425923</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F24" s="14">
         <v>88</v>
@@ -2836,7 +2772,7 @@
     </row>
     <row r="25" spans="1:6" s="16" customFormat="1">
       <c r="A25" s="22" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B25" s="15">
         <v>39762</v>
@@ -2845,10 +2781,10 @@
         <v>39762.999988425923</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>129</v>
+        <v>23</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F25" s="14">
         <v>80</v>
@@ -2856,7 +2792,7 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="22" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B26" s="11">
         <v>39766</v>
@@ -2865,10 +2801,10 @@
         <v>39766.999988425923</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>135</v>
+        <v>24</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F26" s="14">
         <v>89</v>
@@ -2876,7 +2812,7 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="24" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B27" s="11">
         <v>39778</v>
@@ -2885,10 +2821,10 @@
         <v>39778.999884259261</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>107</v>
+        <v>25</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="F27" s="14">
         <v>94</v>
@@ -2896,7 +2832,7 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="25" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="B28" s="11">
         <v>39787</v>
@@ -2905,10 +2841,10 @@
         <v>39787.999988425923</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>111</v>
+        <v>26</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="F28" s="14">
         <v>90</v>
@@ -2916,7 +2852,7 @@
     </row>
     <row r="29" spans="1:6" s="21" customFormat="1">
       <c r="A29" s="23" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="B29" s="20">
         <v>39792</v>
@@ -2925,10 +2861,10 @@
         <v>39792.999988425923</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="F29" s="14">
         <v>40</v>
@@ -2936,7 +2872,7 @@
     </row>
     <row r="30" spans="1:6" s="18" customFormat="1">
       <c r="A30" s="24" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B30" s="17">
         <v>39799</v>
@@ -2945,10 +2881,10 @@
         <v>39799.999988425923</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>119</v>
+        <v>28</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="F30" s="14">
         <v>60</v>
@@ -2956,7 +2892,7 @@
     </row>
     <row r="31" spans="1:6" s="14" customFormat="1">
       <c r="A31" s="24" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="B31" s="13">
         <v>39808</v>
@@ -2965,10 +2901,10 @@
         <v>39808.999988425923</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="F31" s="14">
         <v>80</v>
@@ -2976,7 +2912,7 @@
     </row>
     <row r="32" spans="1:6" s="18" customFormat="1">
       <c r="A32" s="24" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="B32" s="17">
         <v>39818</v>
@@ -2985,10 +2921,10 @@
         <v>39818.999988425923</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="F32" s="14">
         <v>50</v>
@@ -2996,7 +2932,7 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="24" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="B33" s="11">
         <v>39830</v>
@@ -3005,10 +2941,10 @@
         <v>39830.999988425923</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="F33" s="14">
         <v>35</v>
@@ -3016,7 +2952,7 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="24" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="B34" s="11">
         <v>39833</v>
@@ -3025,10 +2961,10 @@
         <v>39833.999988425923</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="F34" s="14">
         <v>95</v>
@@ -3036,7 +2972,7 @@
     </row>
     <row r="35" spans="1:6" s="18" customFormat="1">
       <c r="A35" s="24" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="B35" s="17">
         <v>39835</v>
@@ -3045,10 +2981,10 @@
         <v>39835.999988425923</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="F35" s="14">
         <v>40</v>
@@ -3056,7 +2992,7 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="24" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="B36" s="11">
         <v>39838</v>
@@ -3065,10 +3001,10 @@
         <v>39838.999988425923</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="F36" s="14">
         <v>80</v>
@@ -3076,7 +3012,7 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="22" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="B37" s="11">
         <v>39842</v>
@@ -3085,10 +3021,10 @@
         <v>39842.999988425923</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>75</v>
+        <v>2</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="F37" s="14">
         <v>90</v>
@@ -3102,7 +3038,7 @@
     </row>
     <row r="65" spans="1:5" ht="15">
       <c r="A65" s="7" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="B65" s="11">
         <v>39716</v>
@@ -3111,10 +3047,10 @@
         <v>39716.999884259261</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="E65" s="12" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
make django green, prototype of article processing
</commit_message>
<xml_diff>
--- a/testdata/TimeWire_Events_and_Articles_Spreadsheet.xlsx
+++ b/testdata/TimeWire_Events_and_Articles_Spreadsheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Articles" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="218">
   <si>
     <t>Article_URL</t>
   </si>
@@ -430,15 +430,6 @@
   </si>
   <si>
     <t>http://rt.com/news/israeli-warplanes-bomb-damascus-114/</t>
-  </si>
-  <si>
-    <t>http://eagainst.com/articles/greece-coverage-of-the-september-26-general-strike/</t>
-  </si>
-  <si>
-    <t>http://www.telegraph.co.uk/finance/debt-crisis-live/9566810/Greek-general-strike-and-debt-crisis-as-it-happened-September-26-2012.html</t>
-  </si>
-  <si>
-    <t>http://www.reuters.com/article/2011/09/26/us-greece-idUSTRE78P5ZX20110926</t>
   </si>
   <si>
     <t>Title</t>
@@ -820,15 +811,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>39600</xdr:colOff>
+      <xdr:colOff>66600</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>111960</xdr:rowOff>
+      <xdr:rowOff>61200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>51840</xdr:colOff>
+      <xdr:colOff>78480</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>124200</xdr:rowOff>
+      <xdr:rowOff>73080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -843,8 +834,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="39600" y="2688480"/>
-          <a:ext cx="12240" cy="12240"/>
+          <a:off x="66600" y="2637720"/>
+          <a:ext cx="11880" cy="11880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -863,14 +854,14 @@
   </sheetPr>
   <dimension ref="A1:C128"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B10" activeCellId="0" pane="topLeft" sqref="B10"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A126" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B126" activeCellId="0" pane="topLeft" sqref="B126:B128"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.678431372549"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.6627450980392"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.678431372549"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.7176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.756862745098"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.7176470588235"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="1" s="2">
@@ -1808,23 +1799,17 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="107">
       <c r="C107" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="49.25" outlineLevel="0" r="126">
-      <c r="B126" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="73.1" outlineLevel="0" r="127">
-      <c r="B127" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="37.3" outlineLevel="0" r="128">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="126">
+      <c r="B126" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="127">
+      <c r="B127" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="128">
       <c r="A128" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B128" s="1" t="s">
-        <v>140</v>
-      </c>
+      <c r="B128" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1844,41 +1829,41 @@
   </sheetPr>
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B3" activeCellId="0" pane="topLeft" sqref="B3"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B3" activeCellId="1" pane="topLeft" sqref="B126:B128 B3"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="63.5333333333333"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="6" width="14.6235294117647"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="4" width="53.6274509803922"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="65.1058823529412"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="4" width="10.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="63.7764705882353"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="6" width="14.678431372549"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="4" width="53.8392156862745"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="65.356862745098"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="4" width="10.7882352941176"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1" s="2">
       <c r="A1" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="E1" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="F1" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>146</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="2">
       <c r="A2" s="8" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B2" s="6" t="n">
         <v>39302</v>
@@ -1890,7 +1875,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F2" s="4" t="n">
         <v>50</v>
@@ -1898,7 +1883,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16" outlineLevel="0" r="3">
       <c r="A3" s="8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B3" s="6" t="n">
         <v>39296</v>
@@ -1907,10 +1892,10 @@
         <v>39297.9999884259</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F3" s="4" t="n">
         <v>70</v>
@@ -1918,7 +1903,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="4">
       <c r="A4" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B4" s="6" t="n">
         <v>39357</v>
@@ -1930,7 +1915,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F4" s="4" t="n">
         <v>30</v>
@@ -1938,7 +1923,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="A5" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B5" s="6" t="n">
         <v>39382</v>
@@ -1950,7 +1935,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F5" s="4" t="n">
         <v>80</v>
@@ -1958,7 +1943,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="6">
       <c r="A6" s="9" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B6" s="6" t="n">
         <v>39386</v>
@@ -1970,7 +1955,7 @@
         <v>19</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F6" s="4" t="n">
         <v>72</v>
@@ -1978,7 +1963,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="7">
       <c r="A7" s="9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B7" s="6" t="n">
         <v>39397</v>
@@ -1990,7 +1975,7 @@
         <v>23</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F7" s="4" t="n">
         <v>90</v>
@@ -1998,7 +1983,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="8">
       <c r="A8" s="9" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B8" s="6" t="n">
         <v>39481</v>
@@ -2010,7 +1995,7 @@
         <v>27</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F8" s="4" t="n">
         <v>40</v>
@@ -2018,7 +2003,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="9">
       <c r="A9" s="9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B9" s="6" t="n">
         <v>39499</v>
@@ -2030,7 +2015,7 @@
         <v>31</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F9" s="4" t="n">
         <v>60</v>
@@ -2038,7 +2023,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="A10" s="6" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B10" s="6" t="n">
         <v>39506</v>
@@ -2050,7 +2035,7 @@
         <v>35</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F10" s="4" t="n">
         <v>45</v>
@@ -2058,7 +2043,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="11">
       <c r="A11" s="9" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B11" s="6" t="n">
         <v>39512</v>
@@ -2070,7 +2055,7 @@
         <v>39</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F11" s="4" t="n">
         <v>70</v>
@@ -2078,7 +2063,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13" outlineLevel="0" r="12">
       <c r="A12" s="9" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B12" s="6" t="n">
         <v>39525</v>
@@ -2090,7 +2075,7 @@
         <v>43</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F12" s="4" t="n">
         <v>80</v>
@@ -2098,7 +2083,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="13">
       <c r="A13" s="8" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B13" s="6" t="n">
         <v>39569</v>
@@ -2110,7 +2095,7 @@
         <v>47</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F13" s="4" t="n">
         <v>90</v>
@@ -2118,7 +2103,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="14">
       <c r="A14" s="9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B14" s="6" t="n">
         <v>39648</v>
@@ -2130,7 +2115,7 @@
         <v>51</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F14" s="4" t="n">
         <v>90</v>
@@ -2138,7 +2123,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="15">
       <c r="A15" s="9" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B15" s="6" t="n">
         <v>39685</v>
@@ -2150,7 +2135,7 @@
         <v>55</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F15" s="4" t="n">
         <v>90</v>
@@ -2158,7 +2143,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="16">
       <c r="A16" s="9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B16" s="6" t="n">
         <v>39688</v>
@@ -2167,10 +2152,10 @@
         <v>39688.9999884259</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F16" s="4" t="n">
         <v>85</v>
@@ -2178,7 +2163,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="17">
       <c r="A17" s="9" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B17" s="6" t="n">
         <v>39696</v>
@@ -2190,7 +2175,7 @@
         <v>59</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F17" s="4" t="n">
         <v>80</v>
@@ -2198,7 +2183,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="18">
       <c r="A18" s="9" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B18" s="6" t="n">
         <v>39699</v>
@@ -2210,7 +2195,7 @@
         <v>63</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F18" s="4" t="n">
         <v>85</v>
@@ -2218,7 +2203,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="A19" s="6" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B19" s="6" t="n">
         <v>39705</v>
@@ -2230,7 +2215,7 @@
         <v>67</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F19" s="4" t="n">
         <v>95</v>
@@ -2238,7 +2223,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="20">
       <c r="A20" s="9" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B20" s="6" t="n">
         <v>39724</v>
@@ -2250,7 +2235,7 @@
         <v>71</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F20" s="4" t="n">
         <v>75</v>
@@ -2258,7 +2243,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="21">
       <c r="A21" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B21" s="6" t="n">
         <v>39736</v>
@@ -2270,7 +2255,7 @@
         <v>75</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F21" s="4" t="n">
         <v>60</v>
@@ -2278,7 +2263,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="22">
       <c r="A22" s="8" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B22" s="6" t="n">
         <v>39744</v>
@@ -2290,7 +2275,7 @@
         <v>79</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F22" s="4" t="n">
         <v>92</v>
@@ -2298,7 +2283,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="23">
       <c r="A23" s="9" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B23" s="6" t="n">
         <v>39745</v>
@@ -2310,7 +2295,7 @@
         <v>83</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F23" s="4" t="n">
         <v>88</v>
@@ -2318,7 +2303,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="24">
       <c r="A24" s="8" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B24" s="6" t="n">
         <v>39762</v>
@@ -2330,7 +2315,7 @@
         <v>87</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F24" s="4" t="n">
         <v>80</v>
@@ -2338,7 +2323,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="25">
       <c r="A25" s="8" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B25" s="6" t="n">
         <v>39766</v>
@@ -2350,7 +2335,7 @@
         <v>91</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F25" s="4" t="n">
         <v>89</v>
@@ -2358,7 +2343,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="26">
       <c r="A26" s="9" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B26" s="6" t="n">
         <v>39778</v>
@@ -2370,7 +2355,7 @@
         <v>95</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F26" s="4" t="n">
         <v>94</v>
@@ -2378,7 +2363,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
       <c r="A27" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B27" s="6" t="n">
         <v>39787</v>
@@ -2390,7 +2375,7 @@
         <v>99</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F27" s="4" t="n">
         <v>90</v>
@@ -2398,7 +2383,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
       <c r="A28" s="6" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B28" s="6" t="n">
         <v>39792</v>
@@ -2410,7 +2395,7 @@
         <v>103</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F28" s="4" t="n">
         <v>40</v>
@@ -2418,7 +2403,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="29">
       <c r="A29" s="9" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B29" s="6" t="n">
         <v>39799</v>
@@ -2430,7 +2415,7 @@
         <v>107</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F29" s="4" t="n">
         <v>60</v>
@@ -2438,7 +2423,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="30">
       <c r="A30" s="9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B30" s="6" t="n">
         <v>39808</v>
@@ -2450,7 +2435,7 @@
         <v>111</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F30" s="4" t="n">
         <v>80</v>
@@ -2458,7 +2443,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="31">
       <c r="A31" s="9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B31" s="6" t="n">
         <v>39818</v>
@@ -2470,7 +2455,7 @@
         <v>115</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F31" s="4" t="n">
         <v>50</v>
@@ -2478,7 +2463,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="32">
       <c r="A32" s="9" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B32" s="6" t="n">
         <v>39830</v>
@@ -2490,7 +2475,7 @@
         <v>119</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F32" s="4" t="n">
         <v>35</v>
@@ -2498,7 +2483,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="33">
       <c r="A33" s="9" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B33" s="6" t="n">
         <v>39833</v>
@@ -2510,7 +2495,7 @@
         <v>123</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F33" s="4" t="n">
         <v>95</v>
@@ -2518,7 +2503,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="34">
       <c r="A34" s="9" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B34" s="6" t="n">
         <v>39835</v>
@@ -2530,7 +2515,7 @@
         <v>127</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F34" s="4" t="n">
         <v>40</v>
@@ -2538,7 +2523,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="35">
       <c r="A35" s="9" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B35" s="6" t="n">
         <v>39838</v>
@@ -2550,7 +2535,7 @@
         <v>131</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F35" s="4" t="n">
         <v>80</v>
@@ -2558,7 +2543,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="36">
       <c r="A36" s="8" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B36" s="6" t="n">
         <v>39842</v>
@@ -2570,7 +2555,7 @@
         <v>135</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F36" s="4" t="n">
         <v>90</v>
@@ -2584,7 +2569,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="64">
       <c r="A64" s="11" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B64" s="6" t="n">
         <v>39716</v>
@@ -2593,10 +2578,10 @@
         <v>39716.9998842593</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>